<commit_message>
P2PParser: report bonus payments in a separate column
</commit_message>
<xml_diff>
--- a/tests/expected_results/result_test_download_bondora_statement_no_cfs.xlsx
+++ b/tests/expected_results/result_test_download_bondora_statement_no_cfs.xlsx
@@ -1,111 +1,147 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <workbookProtection/>
-  <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="500" visibility="visible" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
-  </bookViews>
-  <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Data" sheetId="1" state="visible" r:id="rId1"/>
-  </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1" iterate="0" iterateCount="100" iterateDelta="0.0001" refMode="A1"/>
-</workbook>
+<x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:workbookPr codeName="ThisWorkbook"/>
+  <x:bookViews>
+    <x:workbookView firstSheet="0" activeTab="0"/>
+  </x:bookViews>
+  <x:sheets>
+    <x:sheet name="Data" sheetId="2" r:id="rId2"/>
+  </x:sheets>
+  <x:definedNames/>
+  <x:calcPr calcId="125725"/>
+</x:workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <x:si>
+    <x:t>Period</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Opening balance</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Net capital deployed</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Net loan investments</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Principal received - total</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Interest received - total</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Principal and interest received - total</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Closing balance</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Principal planned - total</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Interest planned - total</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Principal and interest planned - total</x:t>
+  </x:si>
+</x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="5">
-    <font>
-      <name val="Calibri"/>
-      <charset val="1"/>
-      <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="11"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="1"/>
-      <family val="2"/>
-      <b val="1"/>
-      <color rgb="FF000000"/>
-      <sz val="11"/>
-    </font>
-  </fonts>
-  <fills count="2">
-    <fill>
-      <patternFill/>
-    </fill>
-    <fill>
-      <patternFill patternType="gray125"/>
-    </fill>
-  </fills>
-  <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-  </borders>
-  <cellStyleXfs count="6">
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-  </cellStyleXfs>
-  <cellXfs count="6">
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="1"/>
-    </xf>
-  </cellXfs>
-  <cellStyles count="6">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" name="Comma" xfId="1"/>
-    <cellStyle builtinId="6" name="Comma [0]" xfId="2"/>
-    <cellStyle builtinId="4" name="Currency" xfId="3"/>
-    <cellStyle builtinId="7" name="Currency [0]" xfId="4"/>
-    <cellStyle builtinId="5" name="Percent" xfId="5"/>
-  </cellStyles>
-</styleSheet>
+<x:styleSheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:numFmts count="1">
+    <x:numFmt numFmtId="0" formatCode=""/>
+  </x:numFmts>
+  <x:fonts count="2">
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+    <x:font>
+      <x:b/>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+  </x:fonts>
+  <x:fills count="2">
+    <x:fill>
+      <x:patternFill patternType="none"/>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="gray125"/>
+    </x:fill>
+  </x:fills>
+  <x:borders count="2">
+    <x:border diagonalUp="0" diagonalDown="0">
+      <x:left style="none">
+        <x:color rgb="FF000000"/>
+      </x:left>
+      <x:right style="none">
+        <x:color rgb="FF000000"/>
+      </x:right>
+      <x:top style="none">
+        <x:color rgb="FF000000"/>
+      </x:top>
+      <x:bottom style="none">
+        <x:color rgb="FF000000"/>
+      </x:bottom>
+      <x:diagonal style="none">
+        <x:color rgb="FF000000"/>
+      </x:diagonal>
+    </x:border>
+    <x:border diagonalUp="0" diagonalDown="0">
+      <x:left style="none">
+        <x:color rgb="FF000000"/>
+      </x:left>
+      <x:right style="none">
+        <x:color rgb="FF000000"/>
+      </x:right>
+      <x:top style="none">
+        <x:color rgb="FF000000"/>
+      </x:top>
+      <x:bottom style="thin">
+        <x:color rgb="FF000000"/>
+      </x:bottom>
+      <x:diagonal style="none">
+        <x:color rgb="FF000000"/>
+      </x:diagonal>
+    </x:border>
+  </x:borders>
+  <x:cellStyleXfs count="2">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+  </x:cellStyleXfs>
+  <x:cellXfs count="2">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+  </x:cellXfs>
+  <x:cellStyles count="1">
+    <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </x:cellStyles>
+</x:styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
@@ -388,94 +424,70 @@
 </a:theme>
 </file>
 
-<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="0">
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="0"/>
-  </sheetPr>
-  <dimension ref="A1:K1"/>
-  <sheetViews>
-    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="G17" activeCellId="0" pane="topLeft" sqref="G17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelRow="0" zeroHeight="0"/>
-  <cols>
-    <col customWidth="1" max="1" min="1" style="3" width="9.74"/>
-    <col customWidth="1" max="2" min="2" style="3" width="14.37"/>
-    <col customWidth="1" max="3" min="3" style="3" width="25.72"/>
-    <col customWidth="1" max="4" min="4" style="3" width="19.85"/>
-    <col customWidth="1" max="5" min="5" style="3" width="31.16"/>
-    <col customWidth="1" max="6" min="6" style="3" width="24.31"/>
-    <col customWidth="1" max="7" min="7" style="3" width="45.62"/>
-    <col customWidth="1" max="8" min="8" style="3" width="9.74"/>
-    <col customWidth="1" max="9" min="9" style="3" width="30.74"/>
-    <col customWidth="1" max="10" min="10" style="3" width="23.88"/>
-    <col customWidth="1" max="11" min="11" style="3" width="39.62"/>
-    <col customWidth="1" max="1025" min="12" style="3" width="8.67"/>
-  </cols>
-  <sheetData>
-    <row customHeight="1" ht="23.85" r="1" s="4">
-      <c r="A1" s="5" t="inlineStr">
-        <is>
-          <t>Period</t>
-        </is>
-      </c>
-      <c r="B1" s="5" t="inlineStr">
-        <is>
-          <t>Opening balance</t>
-        </is>
-      </c>
-      <c r="C1" s="5" t="inlineStr">
-        <is>
-          <t>Net capital deployed</t>
-        </is>
-      </c>
-      <c r="D1" s="5" t="inlineStr">
-        <is>
-          <t>Net loan investments</t>
-        </is>
-      </c>
-      <c r="E1" s="5" t="inlineStr">
-        <is>
-          <t>Principal received - total</t>
-        </is>
-      </c>
-      <c r="F1" s="5" t="inlineStr">
-        <is>
-          <t>Interest received - total</t>
-        </is>
-      </c>
-      <c r="G1" s="5" t="inlineStr">
-        <is>
-          <t>Principal and interest received - total</t>
-        </is>
-      </c>
-      <c r="H1" s="5" t="inlineStr">
-        <is>
-          <t>Closing balance</t>
-        </is>
-      </c>
-      <c r="I1" s="5" t="inlineStr">
-        <is>
-          <t>Principal planned - total</t>
-        </is>
-      </c>
-      <c r="J1" s="5" t="inlineStr">
-        <is>
-          <t>Interest planned - total</t>
-        </is>
-      </c>
-      <c r="K1" s="5" t="inlineStr">
-        <is>
-          <t>Principal and interest planned - total</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
-  <pageMargins bottom="0.5" footer="0.511805555555555" header="0.511805555555555" left="0.75" right="0.75" top="0.75"/>
-  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0" verticalDpi="300"/>
-</worksheet>
+<file path=xl/worksheets/sheet.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:K1"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:cols>
+    <x:col min="1" max="1" width="7.520625" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="16.430625" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="19.890625" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="20.440625" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="23.010625" style="0" customWidth="1"/>
+    <x:col min="6" max="6" width="22.270625" style="0" customWidth="1"/>
+    <x:col min="7" max="7" width="34.020625" style="0" customWidth="1"/>
+    <x:col min="8" max="8" width="15.300625" style="0" customWidth="1"/>
+    <x:col min="9" max="9" width="22.690625" style="0" customWidth="1"/>
+    <x:col min="10" max="10" width="21.960625" style="0" customWidth="1"/>
+    <x:col min="11" max="11" width="33.710625" style="0" customWidth="1"/>
+  </x:cols>
+  <x:sheetData>
+    <x:row r="1" spans="1:11">
+      <x:c r="A1" s="1" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="1" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C1" s="1" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="D1" s="1" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="E1" s="1" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="F1" s="1" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="G1" s="1" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H1" s="1" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="I1" s="1" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="J1" s="1" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="K1" s="1" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
 </file>
</xml_diff>